<commit_message>
Update answers with comments
</commit_message>
<xml_diff>
--- a/out/mia07_t3_tra_resultados_viterbi.xlsx
+++ b/out/mia07_t3_tra_resultados_viterbi.xlsx
@@ -478,11 +478,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>VMIP3S0</t>
+          <t>NCMS000</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0012941074971961</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.01017241781572992</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -509,17 +509,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>DA0MS0</t>
+          <t>VMIP3S0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.0012941074971961</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1398289673695107</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -540,7 +540,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>NCMS000</t>
+          <t>NCMP000</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -553,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01017241781572992</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.0007549414348462665</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -571,7 +571,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Fp</t>
+          <t>AQ0MS0</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.0009827570803180559</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -596,20 +596,20 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0959409594095941</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>SPS00</t>
+          <t>NCFS000</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01959015197765447</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -621,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1249534018034177</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -633,14 +633,14 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>NCMP000</t>
+          <t>SPS00</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.01959015197765447</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -652,10 +652,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.1249534018034177</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0007549414348462665</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -664,7 +664,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>AQ0MS0</t>
+          <t>Fp</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0009827570803180559</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>0.0959409594095941</v>
       </c>
     </row>
     <row r="9">
@@ -726,7 +726,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>NCFS000</t>
+          <t>DA0MS0</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.1398289673695107</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>

</xml_diff>